<commit_message>
Create Contacts Test case updated.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData - NinzaCRM.xlsx
+++ b/src/test/resources/TestData - NinzaCRM.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Integration" sheetId="1" r:id="rId1"/>
     <sheet name="System" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="144">
   <si>
     <t>TC_ID</t>
   </si>
@@ -443,12 +443,21 @@
   </si>
   <si>
     <t>VivoBook Invoice_5</t>
+  </si>
+  <si>
+    <t>TargetSize</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>9876567897</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -505,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -526,6 +535,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -810,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -957,7 +969,9 @@
       <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -989,8 +1003,8 @@
       <c r="D5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="3">
-        <v>9876567897</v>
+      <c r="E5" s="8" t="s">
+        <v>143</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>34</v>
@@ -998,7 +1012,9 @@
       <c r="G5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -2394,6 +2410,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2401,8 +2418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Test Scripts Executed. Batch Script Executed.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData - NinzaCRM.xlsx
+++ b/src/test/resources/TestData - NinzaCRM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="Integration" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="153">
   <si>
     <t>TC_ID</t>
   </si>
@@ -448,10 +448,37 @@
     <t>TargetSize</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>9876567897</t>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>9876543219</t>
+  </si>
+  <si>
+    <t>9876545675</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9876545673</t>
+  </si>
+  <si>
+    <t>500</t>
   </si>
 </sst>
 </file>
@@ -822,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -859,9 +886,15 @@
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -902,9 +935,15 @@
       <c r="H2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="I2" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>148</v>
+      </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
@@ -1004,7 +1043,7 @@
         <v>33</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>34</v>
@@ -1089,7 +1128,7 @@
         <v>24</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>26</v>
@@ -1100,9 +1139,15 @@
       <c r="M7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="N7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -1141,8 +1186,8 @@
       <c r="I8" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="J8" s="3">
-        <v>5000</v>
+      <c r="J8" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>37</v>
@@ -1153,9 +1198,15 @@
       <c r="M8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+      <c r="N8" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>148</v>
+      </c>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
@@ -2419,7 +2470,7 @@
   <dimension ref="A1:AH29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Test cases for Products, Purchase order committed.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData - NinzaCRM.xlsx
+++ b/src/test/resources/TestData - NinzaCRM.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="6450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Integration" sheetId="1" r:id="rId1"/>
     <sheet name="System" sheetId="2" r:id="rId2"/>
+    <sheet name="Functional" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="166">
   <si>
     <t>TC_ID</t>
   </si>
@@ -479,16 +480,62 @@
   </si>
   <si>
     <t>500</t>
+  </si>
+  <si>
+    <t>TC01_Products</t>
+  </si>
+  <si>
+    <t>AddProduct</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Product_123</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>15000</t>
+  </si>
+  <si>
+    <t>75000</t>
+  </si>
+  <si>
+    <t>568989</t>
+  </si>
+  <si>
+    <t>564443</t>
+  </si>
+  <si>
+    <t>9874234789</t>
+  </si>
+  <si>
+    <t>VID_002</t>
+  </si>
+  <si>
+    <t>25-06-2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -541,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,6 +614,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2469,8 +2518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2561,7 +2610,9 @@
       <c r="Z1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AA1" s="1"/>
+      <c r="AA1" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
@@ -2583,8 +2634,8 @@
       <c r="D2" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="3">
-        <v>9876567890</v>
+      <c r="E2" s="8" t="s">
+        <v>163</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>34</v>
@@ -2598,20 +2649,20 @@
       <c r="I2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J2" s="3">
-        <v>10</v>
-      </c>
-      <c r="K2" s="3">
-        <v>75000</v>
+      <c r="J2" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>77</v>
+        <v>164</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="N2" s="5">
-        <v>45918</v>
+      <c r="N2" s="8" t="s">
+        <v>165</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>99</v>
@@ -2625,8 +2676,8 @@
       <c r="R2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="S2" s="3">
-        <v>731204</v>
+      <c r="S2" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>102</v>
@@ -2643,13 +2694,15 @@
       <c r="X2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="3">
-        <v>731204</v>
+      <c r="Y2" s="8" t="s">
+        <v>161</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AA2" s="3"/>
+      <c r="AA2" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
       <c r="AD2" s="3"/>
@@ -4368,5 +4421,97 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" customWidth="1"/>
+    <col min="3" max="3" width="14.36328125" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>